<commit_message>
Get some missing data onto graphs
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/Maricopa/VariableNameMap.xlsx
+++ b/Tests/Validation/Wheat/Maricopa/VariableNameMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\Wheat\Maricopa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFA410A-8B00-4DF4-A716-FFA09BE1BEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999616CF-33E9-4F75-BFF9-418A3FEB70E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2B96E70D-F954-47E5-A8D6-D0402FD709FF}"/>
   </bookViews>
@@ -1520,8 +1520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{120CACDA-B61E-4EB8-BB20-98BB4E7512AF}">
   <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2610,7 +2610,7 @@
         <v>1</v>
       </c>
       <c r="G58">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Fix unit conversion in grain size
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/Maricopa/VariableNameMap.xlsx
+++ b/Tests/Validation/Wheat/Maricopa/VariableNameMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\Wheat\Maricopa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE2C90C-0F1C-40E3-9560-91B435CBF3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D134BE60-DA02-4B22-A82D-93AF222FA3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2B96E70D-F954-47E5-A8D6-D0402FD709FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B96E70D-F954-47E5-A8D6-D0402FD709FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -1520,18 +1520,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{120CACDA-B61E-4EB8-BB20-98BB4E7512AF}">
   <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="H95" sqref="H95"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="G106" sqref="G106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>260</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>258</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>258</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>258</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>258</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>258</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>258</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>258</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>258</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>258</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>258</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>258</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>258</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>258</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>258</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>258</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>258</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>258</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>258</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>258</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>258</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>258</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>258</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>258</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>258</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>258</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>258</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>258</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>258</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>258</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>258</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>258</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>258</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>258</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>258</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>258</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>258</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>258</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>258</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>258</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>258</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>258</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>258</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>258</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>258</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>258</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>258</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>258</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>258</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>258</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>258</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>258</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>258</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>258</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>258</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>258</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>258</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>258</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>258</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>258</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>258</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>258</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>259</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>259</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>259</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>259</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>259</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>259</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>259</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>259</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>259</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>259</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>259</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>259</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>259</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>259</v>
       </c>
@@ -2955,7 +2955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>259</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>259</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>259</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>259</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>259</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>259</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>259</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>259</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>259</v>
       </c>
@@ -3144,7 +3144,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>259</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>259</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>259</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>259</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>259</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>259</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>259</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>259</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>259</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>259</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>259</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>259</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>259</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>259</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>259</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>259</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>259</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>259</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>259</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>259</v>
       </c>
@@ -3577,10 +3577,10 @@
         <v>1</v>
       </c>
       <c r="G105">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>259</v>
       </c>

</xml_diff>